<commit_message>
EditGuis erstellt und implementiert
</commit_message>
<xml_diff>
--- a/Projektjournal Nick.xlsx
+++ b/Projektjournal Nick.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a54f827cd7857792/Desktop/Projektauftrag_Auftragsverwaltung/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick9\source\repos\Projektarbeit-Auftragsverwaltung_Schwerpunktjahr_gui_123\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_AD4DB114E441178AC67DF47D4696E3DE683EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1374E0B-58CD-4880-9322-8435EE41C3EB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C182E6-7049-4D42-BC4F-1D82BC714B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1425" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1425" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>2 Stunden</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Besprechung ERM und Projekt</t>
+  </si>
+  <si>
+    <t>1.5 Stunden</t>
+  </si>
+  <si>
+    <t>Gui erstellen</t>
   </si>
 </sst>
 </file>
@@ -364,15 +370,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -403,6 +412,34 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>44929</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>44930</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>